<commit_message>
Last commit for lab 4. Lamp controller schematic done on paper.
</commit_message>
<xml_diff>
--- a/Lab 4/Part 2 Collector Current Readings.xlsx
+++ b/Lab 4/Part 2 Collector Current Readings.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>VCC</t>
   </si>
@@ -26,13 +26,22 @@
   <si>
     <t>Ic</t>
   </si>
+  <si>
+    <t>Lab 4, Part 2</t>
+  </si>
+  <si>
+    <t>esv and cjd41</t>
+  </si>
+  <si>
+    <t>Edward Venator and Chris Dickey</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="173" formatCode="0.00000"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -65,7 +74,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -210,11 +219,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="45141376"/>
-        <c:axId val="45139840"/>
+        <c:axId val="42866176"/>
+        <c:axId val="42868096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="45141376"/>
+        <c:axId val="42866176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -243,12 +252,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45139840"/>
+        <c:crossAx val="42868096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="45139840"/>
+        <c:axId val="42868096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -278,7 +287,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45141376"/>
+        <c:crossAx val="42866176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -295,7 +304,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -304,16 +313,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>533401</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>171451</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -622,10 +631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,7 +642,7 @@
     <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -643,8 +652,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -659,8 +671,11 @@
         <f>B2*C2</f>
         <v>2.3759075020166716E-7</v>
       </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5</v>
       </c>
@@ -675,8 +690,11 @@
         <f t="shared" ref="D3:D8" si="1">B3*C3</f>
         <v>1.6258889486421083E-2</v>
       </c>
+      <c r="F3" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10.1</v>
       </c>
@@ -692,7 +710,7 @@
         <v>3.4173769830599623E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>15.1</v>
       </c>
@@ -708,7 +726,7 @@
         <v>3.711004302231783E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>20.100000000000001</v>
       </c>
@@ -724,7 +742,7 @@
         <v>3.8216993815541819E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>25</v>
       </c>
@@ -740,7 +758,7 @@
         <v>4.2059760688357088E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>30</v>
       </c>
@@ -758,7 +776,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="0" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>